<commit_message>
Update upper bound for CO2 emissions in 2020
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_2020_Bounds.xlsx
+++ b/SuppXLS/Scen_B_SYS_2020_Bounds.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A27C1A00-5E1F-472C-83D1-32736E6FD69B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79387A36-7EFC-4395-8693-BD4A64EC6241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1605" windowWidth="20520" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -20,9 +20,6 @@
     <sheet name="emi_single" sheetId="18" r:id="rId5"/>
     <sheet name="emi_multi" sheetId="19" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
@@ -1581,15 +1578,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="273">
     <cellStyle name="20% - Accent5 2" xfId="13" xr:uid="{10C4E126-2686-43C7-AD29-7BC90D313B29}"/>
@@ -1946,114 +1943,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Regions"/>
-      <sheetName val="config"/>
-      <sheetName val="single"/>
-      <sheetName val="multi"/>
-      <sheetName val="negative_CO2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="C3" t="str">
-            <v>IE</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>National</v>
-          </cell>
-          <cell r="E3" t="str">
-            <v>IE-CW</v>
-          </cell>
-          <cell r="F3" t="str">
-            <v>IE-D</v>
-          </cell>
-          <cell r="G3" t="str">
-            <v>IE-KE</v>
-          </cell>
-          <cell r="H3" t="str">
-            <v>IE-KK</v>
-          </cell>
-          <cell r="I3" t="str">
-            <v>IE-LS</v>
-          </cell>
-          <cell r="J3" t="str">
-            <v>IE-LD</v>
-          </cell>
-          <cell r="K3" t="str">
-            <v>IE-LH</v>
-          </cell>
-          <cell r="L3" t="str">
-            <v>IE-MH</v>
-          </cell>
-          <cell r="M3" t="str">
-            <v>IE-OY</v>
-          </cell>
-          <cell r="N3" t="str">
-            <v>IE-WH</v>
-          </cell>
-          <cell r="O3" t="str">
-            <v>IE-WX</v>
-          </cell>
-          <cell r="P3" t="str">
-            <v>IE-WW</v>
-          </cell>
-          <cell r="Q3" t="str">
-            <v>IE-CE</v>
-          </cell>
-          <cell r="R3" t="str">
-            <v>IE-CO</v>
-          </cell>
-          <cell r="S3" t="str">
-            <v>IE-KY</v>
-          </cell>
-          <cell r="T3" t="str">
-            <v>IE-LK</v>
-          </cell>
-          <cell r="U3" t="str">
-            <v>IE-TA</v>
-          </cell>
-          <cell r="V3" t="str">
-            <v>IE-WD</v>
-          </cell>
-          <cell r="W3" t="str">
-            <v>IE-G</v>
-          </cell>
-          <cell r="X3" t="str">
-            <v>IE-LM</v>
-          </cell>
-          <cell r="Y3" t="str">
-            <v>IE-MO</v>
-          </cell>
-          <cell r="Z3" t="str">
-            <v>IE-RN</v>
-          </cell>
-          <cell r="AA3" t="str">
-            <v>IE-SO</v>
-          </cell>
-          <cell r="AB3" t="str">
-            <v>IE-CN</v>
-          </cell>
-          <cell r="AC3" t="str">
-            <v>IE-DL</v>
-          </cell>
-          <cell r="AD3" t="str">
-            <v>IE-MN</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2377,7 +2266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8641EA-1C7A-4D34-A01F-F78117DFF5FC}">
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
@@ -3170,7 +3059,7 @@
   <dimension ref="A1:AH24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5284,10 +5173,10 @@
       <c r="AC44" s="28"/>
     </row>
     <row r="49" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B49" s="44" t="s">
+      <c r="B49" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C49" s="44"/>
+      <c r="C49" s="50"/>
     </row>
     <row r="50" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="34" t="s">
@@ -5921,8 +5810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E894F25-B177-4255-B4D5-BD4DFEB7A0BB}">
   <dimension ref="B4:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5969,8 +5858,8 @@
       <c r="B7" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="C7" s="19">
-        <v>35044</v>
+      <c r="C7" s="24">
+        <v>33792</v>
       </c>
       <c r="D7" s="19">
         <v>1</v>
@@ -6031,7 +5920,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6065,13 +5954,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="str">
-        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!C3)</f>
+      <c r="B2" s="44" t="str">
+        <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6082,34 +5971,34 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="45" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6127,7 +6016,7 @@
       <c r="J6" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="K6" s="50"/>
+      <c r="K6" s="49"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="str">
@@ -6155,7 +6044,7 @@
       </c>
       <c r="J7" s="19">
         <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
-        <v>35044</v>
+        <v>33792</v>
       </c>
       <c r="K7" s="19" t="str">
         <f>VLOOKUP(K$5, emi_config!$B$4:$D$14,2,FALSE) &amp; " - Single"</f>
@@ -6229,13 +6118,13 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="45" t="str">
-        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,[1]Regions!D3:AD3)</f>
-        <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      <c r="B2" s="44" t="str">
+        <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
+        <v>~UC_Sets: R_S: IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>257</v>
       </c>
     </row>
@@ -6246,34 +6135,34 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="46" t="s">
         <v>248</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>250</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="47" t="s">
         <v>255</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="47" t="s">
         <v>254</v>
       </c>
-      <c r="J5" s="49" t="s">
+      <c r="J5" s="48" t="s">
         <v>263</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="45" t="s">
         <v>259</v>
       </c>
     </row>
@@ -6319,7 +6208,7 @@
       </c>
       <c r="J7" s="19">
         <f>VLOOKUP("Value", emi_config!$B$4:$D$14,MATCH($F7,emi_config!$B$6:$D$6,),FALSE)</f>
-        <v>35044</v>
+        <v>33792</v>
       </c>
       <c r="K7" s="19" t="str">
         <f>VLOOKUP(K$5, emi_config!$B$4:$D$14,2,FALSE) &amp; " - Multi"</f>

</xml_diff>